<commit_message>
Added missing results for Enrymar Cisneros
</commit_message>
<xml_diff>
--- a/data/2021-12-27/SCW Weekly Comp 2021-12-27 (Responses).xlsx
+++ b/data/2021-12-27/SCW Weekly Comp 2021-12-27 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="226">
   <si>
     <t>Timestamp</t>
   </si>
@@ -593,6 +593,102 @@
   </si>
   <si>
     <t>2:03.57</t>
+  </si>
+  <si>
+    <t>Enrymar Cisneros</t>
+  </si>
+  <si>
+    <t>2013CISN01</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/343359980546742/?post_id=350246939858046&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>1:34.36</t>
+  </si>
+  <si>
+    <t>1:42.12</t>
+  </si>
+  <si>
+    <t>1:39.64</t>
+  </si>
+  <si>
+    <t>1:38.92</t>
+  </si>
+  <si>
+    <t>1:36.72</t>
+  </si>
+  <si>
+    <t>1:38.43</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/343359980546742/?post_id=350165623199511&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/343359980546742/?post_id=350163353199738&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1083505512394794/?post_id=1091527064925972&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1083505512394794/?post_id=1091524834926195&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/364077578855426/?post_id=371890168074167&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>5:45.96</t>
+  </si>
+  <si>
+    <t>5:25.99</t>
+  </si>
+  <si>
+    <t>5:40.08</t>
+  </si>
+  <si>
+    <t>5:37.34</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/364077578855426/?post_id=371704864759364&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>3:40.63</t>
+  </si>
+  <si>
+    <t>3:39.47</t>
+  </si>
+  <si>
+    <t>3:22.95</t>
+  </si>
+  <si>
+    <t>3:34.35</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/364077578855426/?post_id=371693138093870&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>1:06.77</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/364077578855426/?post_id=371689508094233&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>1:56.90</t>
+  </si>
+  <si>
+    <t>1:45.00</t>
+  </si>
+  <si>
+    <t>1:46.67</t>
+  </si>
+  <si>
+    <t>1:52.90</t>
+  </si>
+  <si>
+    <t>1:47.39</t>
+  </si>
+  <si>
+    <t>1:48.99</t>
   </si>
 </sst>
 </file>
@@ -3142,6 +3238,363 @@
         <v>70</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>44571.71661831018</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA51" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="BB51" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC51" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="BD51" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="BE51" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="BF51" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="BG51" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>44571.71736016204</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H52" s="3">
+        <v>4.74</v>
+      </c>
+      <c r="I52" s="3">
+        <v>8.17</v>
+      </c>
+      <c r="J52" s="3">
+        <v>5.35</v>
+      </c>
+      <c r="K52" s="3">
+        <v>5.87</v>
+      </c>
+      <c r="L52" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="M52" s="3">
+        <v>4.74</v>
+      </c>
+      <c r="N52" s="3">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2">
+        <v>44571.71794107639</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O53" s="3">
+        <v>12.35</v>
+      </c>
+      <c r="P53" s="3">
+        <v>13.93</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>12.61</v>
+      </c>
+      <c r="R53" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="S53" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="T53" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="U53" s="3">
+        <v>12.39</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>44571.719053622684</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH54" s="3">
+        <v>9.2</v>
+      </c>
+      <c r="BI54" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="BJ54" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="BK54" s="3">
+        <v>9.53</v>
+      </c>
+      <c r="BL54" s="3">
+        <v>5.99</v>
+      </c>
+      <c r="BM54" s="3">
+        <v>5.99</v>
+      </c>
+      <c r="BN54" s="3">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>44571.72001913194</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO55" s="3">
+        <v>3.85</v>
+      </c>
+      <c r="BP55" s="3">
+        <v>13.41</v>
+      </c>
+      <c r="BQ55" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="BR55" s="3">
+        <v>8.49</v>
+      </c>
+      <c r="BS55" s="3">
+        <v>8.61</v>
+      </c>
+      <c r="BT55" s="3">
+        <v>3.85</v>
+      </c>
+      <c r="BU55" s="3">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>44571.72069488426</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AO56" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AP56" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AQ56" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR56" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS56" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>44571.72126261574</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ57" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK57" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL57" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM57" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN57" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>44571.7220156713</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="V58" s="3">
+        <v>53.59</v>
+      </c>
+      <c r="W58" s="3">
+        <v>51.09</v>
+      </c>
+      <c r="X58" s="3">
+        <v>52.06</v>
+      </c>
+      <c r="Y58" s="3">
+        <v>54.0</v>
+      </c>
+      <c r="Z58" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA58" s="3">
+        <v>51.09</v>
+      </c>
+      <c r="AB58" s="3">
+        <v>53.22</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>44571.722717743054</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC59" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD59" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AE59" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF59" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG59" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH59" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AI59" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
@@ -3193,7 +3646,16 @@
     <hyperlink r:id="rId47" ref="F48"/>
     <hyperlink r:id="rId48" ref="F49"/>
     <hyperlink r:id="rId49" ref="F50"/>
+    <hyperlink r:id="rId50" ref="F51"/>
+    <hyperlink r:id="rId51" ref="F52"/>
+    <hyperlink r:id="rId52" ref="F53"/>
+    <hyperlink r:id="rId53" ref="F54"/>
+    <hyperlink r:id="rId54" ref="F55"/>
+    <hyperlink r:id="rId55" ref="F56"/>
+    <hyperlink r:id="rId56" ref="F57"/>
+    <hyperlink r:id="rId57" ref="F58"/>
+    <hyperlink r:id="rId58" ref="F59"/>
   </hyperlinks>
-  <drawing r:id="rId50"/>
+  <drawing r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>